<commit_message>
some changes to the traces
</commit_message>
<xml_diff>
--- a/Documentation/BillOfMaterials.xlsx
+++ b/Documentation/BillOfMaterials.xlsx
@@ -4,18 +4,14 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1875" yWindow="0" windowWidth="21840" windowHeight="13740" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="1875" yWindow="0" windowWidth="17325" windowHeight="9450" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Revision Control" sheetId="2" r:id="rId1"/>
     <sheet name="BOM" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="145621" concurrentCalc="0"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
-    </ext>
-  </extLst>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
@@ -362,9 +358,6 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -734,11 +727,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -747,7 +735,7 @@
   <dimension ref="A1:I41"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -806,7 +794,7 @@
         <v>1.29</v>
       </c>
       <c r="F2" s="3">
-        <f t="shared" ref="F2" si="0">C2*E2</f>
+        <f>C2*E2</f>
         <v>1.29</v>
       </c>
       <c r="H2">
@@ -861,7 +849,7 @@
         <v>0.83</v>
       </c>
       <c r="F5" s="3">
-        <f t="shared" ref="F5:F40" si="1">C5*E5</f>
+        <f t="shared" ref="F5:F40" si="0">C5*E5</f>
         <v>1.66</v>
       </c>
     </row>
@@ -879,7 +867,7 @@
         <v>0.67</v>
       </c>
       <c r="F6" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>1.34</v>
       </c>
     </row>
@@ -897,7 +885,7 @@
         <v>0.78</v>
       </c>
       <c r="F7" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>1.56</v>
       </c>
     </row>
@@ -915,7 +903,7 @@
         <v>9.94</v>
       </c>
       <c r="F8" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>9.94</v>
       </c>
     </row>
@@ -933,7 +921,7 @@
         <v>2.93</v>
       </c>
       <c r="F9" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>2.93</v>
       </c>
     </row>
@@ -951,7 +939,7 @@
         <v>4.16</v>
       </c>
       <c r="F10" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>4.16</v>
       </c>
     </row>
@@ -969,7 +957,7 @@
         <v>2.75</v>
       </c>
       <c r="F11" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>2.75</v>
       </c>
     </row>
@@ -997,7 +985,7 @@
         <v>0.6</v>
       </c>
       <c r="F13" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>1.2</v>
       </c>
     </row>
@@ -1015,7 +1003,7 @@
         <v>0.46</v>
       </c>
       <c r="F14" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>2.3000000000000003</v>
       </c>
     </row>
@@ -1033,7 +1021,7 @@
         <v>0.63</v>
       </c>
       <c r="F15" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>1.26</v>
       </c>
     </row>
@@ -1051,7 +1039,7 @@
         <v>0.49</v>
       </c>
       <c r="F16" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0.98</v>
       </c>
     </row>
@@ -1069,7 +1057,7 @@
         <v>0.51</v>
       </c>
       <c r="F17" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>2.04</v>
       </c>
     </row>
@@ -1087,7 +1075,7 @@
         <v>5.61</v>
       </c>
       <c r="F18" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>5.61</v>
       </c>
     </row>
@@ -1114,7 +1102,7 @@
         <v>0.1</v>
       </c>
       <c r="F20" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0.1</v>
       </c>
     </row>
@@ -1132,7 +1120,7 @@
         <v>4.13</v>
       </c>
       <c r="F21" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>4.13</v>
       </c>
     </row>
@@ -1150,7 +1138,7 @@
         <v>0.59</v>
       </c>
       <c r="F22" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0.59</v>
       </c>
     </row>
@@ -1168,7 +1156,7 @@
         <v>4.2</v>
       </c>
       <c r="F23" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>8.4</v>
       </c>
     </row>
@@ -1186,7 +1174,7 @@
         <v>0.1</v>
       </c>
       <c r="F24" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>2.1</v>
       </c>
     </row>
@@ -1204,7 +1192,7 @@
         <v>0.1</v>
       </c>
       <c r="F25" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0.4</v>
       </c>
     </row>
@@ -1222,7 +1210,7 @@
         <v>0.95</v>
       </c>
       <c r="F26" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>1.9</v>
       </c>
     </row>
@@ -1240,7 +1228,7 @@
         <v>0.2</v>
       </c>
       <c r="F27" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0.4</v>
       </c>
     </row>
@@ -1268,7 +1256,7 @@
         <v>1.76</v>
       </c>
       <c r="F29" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>1.76</v>
       </c>
     </row>
@@ -1286,7 +1274,7 @@
         <v>3.13</v>
       </c>
       <c r="F30" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>3.13</v>
       </c>
     </row>
@@ -1304,7 +1292,7 @@
         <v>0.81</v>
       </c>
       <c r="F31" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>2.4300000000000002</v>
       </c>
     </row>
@@ -1322,7 +1310,7 @@
         <v>0.21</v>
       </c>
       <c r="F32" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0.63</v>
       </c>
     </row>
@@ -1340,7 +1328,7 @@
         <v>0.46</v>
       </c>
       <c r="F33" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0.92</v>
       </c>
     </row>
@@ -1358,7 +1346,7 @@
         <v>0.1</v>
       </c>
       <c r="F34" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0.1</v>
       </c>
     </row>
@@ -1376,7 +1364,7 @@
         <v>0.19</v>
       </c>
       <c r="F35" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0.19</v>
       </c>
     </row>
@@ -1394,7 +1382,7 @@
         <v>0.1</v>
       </c>
       <c r="F36" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0.1</v>
       </c>
     </row>
@@ -1412,7 +1400,7 @@
         <v>0.1</v>
       </c>
       <c r="F37" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0.1</v>
       </c>
     </row>
@@ -1430,7 +1418,7 @@
         <v>0.1</v>
       </c>
       <c r="F38" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0.1</v>
       </c>
     </row>
@@ -1448,7 +1436,7 @@
         <v>0.43</v>
       </c>
       <c r="F39" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0.43</v>
       </c>
     </row>
@@ -1466,7 +1454,7 @@
         <v>0.1</v>
       </c>
       <c r="F40" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0.1</v>
       </c>
     </row>
@@ -1515,10 +1503,5 @@
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId35"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>